<commit_message>
Update DEMANDA DE SERVICIOS DEL ISTP ALFREDO SARMIENTO PALOMINO.xlsx
</commit_message>
<xml_diff>
--- a/CALCULOS DE DEMANDA/DEMANDA DE SERVICIOS DEL ISTP ALFREDO SARMIENTO PALOMINO.xlsx
+++ b/CALCULOS DE DEMANDA/DEMANDA DE SERVICIOS DEL ISTP ALFREDO SARMIENTO PALOMINO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\REPOSITORIO ORFEI\PROYECTO-035\CALCULOS DE DEMANDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C6EDEF-6B2C-450B-9D2D-2174E1797700}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F4A089-3372-481B-9B01-28C4EE386A66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{35FB2B50-CCB2-49E2-8EB9-1608D8A05A77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="384">
   <si>
     <t>AREA # 030204</t>
   </si>
@@ -1175,6 +1175,66 @@
   <si>
     <t>Tasa prom. Participación matriculas</t>
   </si>
+  <si>
+    <t>POSTULANTES AL INSTITUTO SUPERIOR TECNOLOGICA PUBLICA ALFREDO SARMIENTO PALOMINO</t>
+  </si>
+  <si>
+    <t>Total Postulantes (*)</t>
+  </si>
+  <si>
+    <t>Tasa geométrica</t>
+  </si>
+  <si>
+    <t>años</t>
+  </si>
+  <si>
+    <t>Tasa de crecimiento histórico Const. Civil</t>
+  </si>
+  <si>
+    <t>Tasa de crecimiento histórico Industria Alimentarias</t>
+  </si>
+  <si>
+    <t>POBLACIÓN DE REFERENCIA PROYECTADA</t>
+  </si>
+  <si>
+    <t>CARRERA DE INDUSTRIAS ALIMENTARIAS</t>
+  </si>
+  <si>
+    <t>Población de Referencia</t>
+  </si>
+  <si>
+    <t>periodo o</t>
+  </si>
+  <si>
+    <t>Per. 1</t>
+  </si>
+  <si>
+    <t>Per. 2</t>
+  </si>
+  <si>
+    <t>Per. 3</t>
+  </si>
+  <si>
+    <t>Per. 4</t>
+  </si>
+  <si>
+    <t>Per. 5</t>
+  </si>
+  <si>
+    <t>Per. 6</t>
+  </si>
+  <si>
+    <t>Per. 7</t>
+  </si>
+  <si>
+    <t>Per. 8</t>
+  </si>
+  <si>
+    <t>Per. 9</t>
+  </si>
+  <si>
+    <t>Per. 10</t>
+  </si>
 </sst>
 </file>
 
@@ -1185,7 +1245,7 @@
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1436,8 +1496,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1543,6 +1608,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2199,7 +2276,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="237">
+  <cellXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2650,6 +2727,78 @@
     <xf numFmtId="1" fontId="34" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="17" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="15" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2665,67 +2814,133 @@
     <xf numFmtId="3" fontId="15" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2755,154 +2970,66 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="17" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="15" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4623,7 +4750,7 @@
   <dimension ref="A2:N139"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118"/>
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -4643,7 +4770,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K2" s="152" t="s">
+      <c r="K2" s="176" t="s">
         <v>209</v>
       </c>
       <c r="L2" s="22" t="s">
@@ -4654,7 +4781,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="K3" s="152"/>
+      <c r="K3" s="176"/>
       <c r="L3" s="22" t="s">
         <v>212</v>
       </c>
@@ -4666,7 +4793,7 @@
       <c r="A4" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="K4" s="152"/>
+      <c r="K4" s="176"/>
       <c r="L4" s="22" t="s">
         <v>214</v>
       </c>
@@ -4691,7 +4818,7 @@
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
-      <c r="K5" s="152"/>
+      <c r="K5" s="176"/>
       <c r="L5" s="22" t="s">
         <v>216</v>
       </c>
@@ -4708,7 +4835,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
-      <c r="K6" s="152"/>
+      <c r="K6" s="176"/>
       <c r="L6" s="28" t="s">
         <v>206</v>
       </c>
@@ -4777,7 +4904,7 @@
       <c r="I8" s="17">
         <v>1.12220641997528E-2</v>
       </c>
-      <c r="K8" s="155" t="s">
+      <c r="K8" s="179" t="s">
         <v>218</v>
       </c>
       <c r="L8" s="23" t="s">
@@ -4812,7 +4939,7 @@
       <c r="I9" s="17">
         <v>2.42809808578364E-2</v>
       </c>
-      <c r="K9" s="155"/>
+      <c r="K9" s="179"/>
       <c r="L9" s="25">
         <v>1</v>
       </c>
@@ -4845,7 +4972,7 @@
       <c r="I10" s="17">
         <v>4.0534224964335598E-2</v>
       </c>
-      <c r="K10" s="155"/>
+      <c r="K10" s="179"/>
       <c r="L10" s="25">
         <v>2</v>
       </c>
@@ -4878,7 +5005,7 @@
       <c r="I11" s="17">
         <v>5.7216414936108302E-2</v>
       </c>
-      <c r="K11" s="155"/>
+      <c r="K11" s="179"/>
       <c r="L11" s="25">
         <v>3</v>
       </c>
@@ -4911,7 +5038,7 @@
       <c r="I12" s="17">
         <v>7.2493294998307006E-2</v>
       </c>
-      <c r="K12" s="155"/>
+      <c r="K12" s="179"/>
       <c r="L12" s="25">
         <v>4</v>
       </c>
@@ -4944,7 +5071,7 @@
       <c r="I13" s="17">
         <v>9.2429521932332101E-2</v>
       </c>
-      <c r="K13" s="155"/>
+      <c r="K13" s="179"/>
       <c r="L13" s="25">
         <v>5</v>
       </c>
@@ -4977,7 +5104,7 @@
       <c r="I14" s="17">
         <v>0.110458072549454</v>
       </c>
-      <c r="K14" s="155"/>
+      <c r="K14" s="179"/>
       <c r="L14" s="25">
         <v>6</v>
       </c>
@@ -5010,7 +5137,7 @@
       <c r="I15" s="17">
         <v>0.13315095229583701</v>
       </c>
-      <c r="K15" s="155"/>
+      <c r="K15" s="179"/>
       <c r="L15" s="25">
         <v>7</v>
       </c>
@@ -5043,7 +5170,7 @@
       <c r="I16" s="17">
         <v>0.15706523080858101</v>
       </c>
-      <c r="K16" s="155"/>
+      <c r="K16" s="179"/>
       <c r="L16" s="25">
         <v>8</v>
       </c>
@@ -5076,7 +5203,7 @@
       <c r="I17" s="17">
         <v>0.17786366584129401</v>
       </c>
-      <c r="K17" s="155"/>
+      <c r="K17" s="179"/>
       <c r="L17" s="25">
         <v>9</v>
       </c>
@@ -5109,7 +5236,7 @@
       <c r="I18" s="17">
         <v>0.19936728181294999</v>
       </c>
-      <c r="K18" s="155"/>
+      <c r="K18" s="179"/>
       <c r="L18" s="25">
         <v>10</v>
       </c>
@@ -5142,7 +5269,7 @@
       <c r="I19" s="17">
         <v>0.22272622006005399</v>
       </c>
-      <c r="K19" s="155"/>
+      <c r="K19" s="179"/>
       <c r="L19" s="25">
         <v>11</v>
       </c>
@@ -5175,7 +5302,7 @@
       <c r="I20" s="17">
         <v>0.24853967233204699</v>
       </c>
-      <c r="K20" s="155"/>
+      <c r="K20" s="179"/>
       <c r="L20" s="25">
         <v>12</v>
       </c>
@@ -5208,7 +5335,7 @@
       <c r="I21" s="17">
         <v>0.27281756444609701</v>
       </c>
-      <c r="K21" s="155"/>
+      <c r="K21" s="179"/>
       <c r="L21" s="25">
         <v>13</v>
       </c>
@@ -5241,7 +5368,7 @@
       <c r="I22" s="17">
         <v>0.29411892827154901</v>
       </c>
-      <c r="K22" s="155"/>
+      <c r="K22" s="179"/>
       <c r="L22" s="25">
         <v>14</v>
       </c>
@@ -5274,7 +5401,7 @@
       <c r="I23" s="17">
         <v>0.31491634238404698</v>
       </c>
-      <c r="K23" s="155"/>
+      <c r="K23" s="179"/>
       <c r="L23" s="25">
         <v>15</v>
       </c>
@@ -5307,7 +5434,7 @@
       <c r="I24" s="17">
         <v>0.33519476776427998</v>
       </c>
-      <c r="K24" s="155"/>
+      <c r="K24" s="179"/>
       <c r="L24" s="25">
         <v>16</v>
       </c>
@@ -5340,7 +5467,7 @@
       <c r="I25" s="17">
         <v>0.35314484572600202</v>
       </c>
-      <c r="K25" s="155"/>
+      <c r="K25" s="179"/>
       <c r="L25" s="25">
         <v>17</v>
       </c>
@@ -5373,7 +5500,7 @@
       <c r="I26" s="17">
         <v>0.368667589937197</v>
       </c>
-      <c r="K26" s="155"/>
+      <c r="K26" s="179"/>
       <c r="L26" s="25">
         <v>18</v>
       </c>
@@ -5406,7 +5533,7 @@
       <c r="I27" s="17">
         <v>0.38110756456661499</v>
       </c>
-      <c r="K27" s="155"/>
+      <c r="K27" s="179"/>
       <c r="L27" s="25">
         <v>19</v>
       </c>
@@ -5439,7 +5566,7 @@
       <c r="I28" s="17">
         <v>0.39552916583221398</v>
       </c>
-      <c r="K28" s="156" t="s">
+      <c r="K28" s="180" t="s">
         <v>220</v>
       </c>
       <c r="L28" s="26" t="s">
@@ -5474,7 +5601,7 @@
       <c r="I29" s="17">
         <v>0.405698283610674</v>
       </c>
-      <c r="K29" s="156"/>
+      <c r="K29" s="180"/>
       <c r="L29" s="26" t="s">
         <v>222</v>
       </c>
@@ -5507,7 +5634,7 @@
       <c r="I30" s="17">
         <v>0.41896690541231102</v>
       </c>
-      <c r="K30" s="156"/>
+      <c r="K30" s="180"/>
       <c r="L30" s="26" t="s">
         <v>223</v>
       </c>
@@ -5540,7 +5667,7 @@
       <c r="I31" s="17">
         <v>0.43100154121860501</v>
       </c>
-      <c r="K31" s="156"/>
+      <c r="K31" s="180"/>
       <c r="L31" s="26" t="s">
         <v>224</v>
       </c>
@@ -5573,7 +5700,7 @@
       <c r="I32" s="17">
         <v>0.442984309022109</v>
       </c>
-      <c r="K32" s="156"/>
+      <c r="K32" s="180"/>
       <c r="L32" s="26" t="s">
         <v>225</v>
       </c>
@@ -5606,7 +5733,7 @@
       <c r="I33" s="17">
         <v>0.45545824821289499</v>
       </c>
-      <c r="K33" s="156"/>
+      <c r="K33" s="180"/>
       <c r="L33" s="26" t="s">
         <v>226</v>
       </c>
@@ -5639,7 +5766,7 @@
       <c r="I34" s="17">
         <v>0.46322084753672299</v>
       </c>
-      <c r="K34" s="156"/>
+      <c r="K34" s="180"/>
       <c r="L34" s="26" t="s">
         <v>227</v>
       </c>
@@ -5672,7 +5799,7 @@
       <c r="I35" s="17">
         <v>0.47464392966994801</v>
       </c>
-      <c r="K35" s="156"/>
+      <c r="K35" s="180"/>
       <c r="L35" s="26" t="s">
         <v>228</v>
       </c>
@@ -5705,7 +5832,7 @@
       <c r="I36" s="17">
         <v>0.484015124043298</v>
       </c>
-      <c r="K36" s="156"/>
+      <c r="K36" s="180"/>
       <c r="L36" s="26" t="s">
         <v>229</v>
       </c>
@@ -5738,7 +5865,7 @@
       <c r="I37" s="17">
         <v>0.49526944192962802</v>
       </c>
-      <c r="K37" s="156"/>
+      <c r="K37" s="180"/>
       <c r="L37" s="26" t="s">
         <v>230</v>
       </c>
@@ -5771,7 +5898,7 @@
       <c r="I38" s="17">
         <v>0.50593192354971295</v>
       </c>
-      <c r="K38" s="156"/>
+      <c r="K38" s="180"/>
       <c r="L38" s="26" t="s">
         <v>231</v>
       </c>
@@ -5804,7 +5931,7 @@
       <c r="I39" s="17">
         <v>0.51779485865617103</v>
       </c>
-      <c r="K39" s="156"/>
+      <c r="K39" s="180"/>
       <c r="L39" s="26" t="s">
         <v>232</v>
       </c>
@@ -5837,7 +5964,7 @@
       <c r="I40" s="17">
         <v>0.52978976268593903</v>
       </c>
-      <c r="K40" s="156"/>
+      <c r="K40" s="180"/>
       <c r="L40" s="26" t="s">
         <v>233</v>
       </c>
@@ -7561,13 +7688,13 @@
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="153" t="s">
+      <c r="A107" s="177" t="s">
         <v>241</v>
       </c>
-      <c r="B107" s="154"/>
-      <c r="C107" s="154"/>
-      <c r="D107" s="154"/>
-      <c r="E107" s="154"/>
+      <c r="B107" s="178"/>
+      <c r="C107" s="178"/>
+      <c r="D107" s="178"/>
+      <c r="E107" s="178"/>
       <c r="F107" s="42" t="s">
         <v>206</v>
       </c>
@@ -7582,31 +7709,31 @@
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A108" s="153" t="s">
+      <c r="A108" s="177" t="s">
         <v>240</v>
       </c>
-      <c r="B108" s="154"/>
-      <c r="C108" s="154"/>
-      <c r="D108" s="154"/>
-      <c r="E108" s="154"/>
+      <c r="B108" s="178"/>
+      <c r="C108" s="178"/>
+      <c r="D108" s="178"/>
+      <c r="E108" s="178"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F109" s="153" t="s">
+      <c r="F109" s="177" t="s">
         <v>239</v>
       </c>
-      <c r="G109" s="154"/>
-      <c r="H109" s="154"/>
-      <c r="I109" s="154"/>
-      <c r="J109" s="154"/>
+      <c r="G109" s="178"/>
+      <c r="H109" s="178"/>
+      <c r="I109" s="178"/>
+      <c r="J109" s="178"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F110" s="153" t="s">
+      <c r="F110" s="177" t="s">
         <v>240</v>
       </c>
-      <c r="G110" s="154"/>
-      <c r="H110" s="154"/>
-      <c r="I110" s="154"/>
-      <c r="J110" s="154"/>
+      <c r="G110" s="178"/>
+      <c r="H110" s="178"/>
+      <c r="I110" s="178"/>
+      <c r="J110" s="178"/>
     </row>
     <row r="114" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A114" s="56" t="s">
@@ -7648,27 +7775,27 @@
       </c>
     </row>
     <row r="117" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="157" t="s">
+      <c r="A117" s="168" t="s">
         <v>255</v>
       </c>
-      <c r="B117" s="162" t="s">
+      <c r="B117" s="173" t="s">
         <v>278</v>
       </c>
-      <c r="C117" s="163"/>
-      <c r="D117" s="163"/>
-      <c r="E117" s="163"/>
-      <c r="F117" s="163"/>
-      <c r="G117" s="163"/>
-      <c r="H117" s="163"/>
-      <c r="I117" s="163"/>
-      <c r="J117" s="163"/>
-      <c r="K117" s="163"/>
-      <c r="L117" s="163"/>
-      <c r="M117" s="163"/>
-      <c r="N117" s="164"/>
+      <c r="C117" s="174"/>
+      <c r="D117" s="174"/>
+      <c r="E117" s="174"/>
+      <c r="F117" s="174"/>
+      <c r="G117" s="174"/>
+      <c r="H117" s="174"/>
+      <c r="I117" s="174"/>
+      <c r="J117" s="174"/>
+      <c r="K117" s="174"/>
+      <c r="L117" s="174"/>
+      <c r="M117" s="174"/>
+      <c r="N117" s="175"/>
     </row>
     <row r="118" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="157"/>
+      <c r="A118" s="168"/>
       <c r="B118" s="53">
         <v>2019</v>
       </c>
@@ -7722,12 +7849,12 @@
       </c>
     </row>
     <row r="119" spans="1:14" ht="34.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="157"/>
-      <c r="B119" s="159" t="s">
+      <c r="A119" s="168"/>
+      <c r="B119" s="170" t="s">
         <v>277</v>
       </c>
-      <c r="C119" s="160"/>
-      <c r="D119" s="161"/>
+      <c r="C119" s="171"/>
+      <c r="D119" s="172"/>
       <c r="E119" s="54" t="s">
         <v>245</v>
       </c>
@@ -7855,7 +7982,7 @@
       <c r="B126" s="46">
         <v>488</v>
       </c>
-      <c r="C126" s="158">
+      <c r="C126" s="169">
         <v>0.32675410103003655</v>
       </c>
       <c r="D126" s="49">
@@ -7868,7 +7995,7 @@
       <c r="G126" s="46">
         <v>640</v>
       </c>
-      <c r="H126" s="158">
+      <c r="H126" s="169">
         <v>0.32475247524752476</v>
       </c>
       <c r="I126" s="49">
@@ -7883,7 +8010,7 @@
       <c r="B127" s="46">
         <v>363</v>
       </c>
-      <c r="C127" s="158"/>
+      <c r="C127" s="169"/>
       <c r="D127" s="49">
         <f t="shared" ref="D127:D135" si="2">B127*$C$126</f>
         <v>118.61173867390326</v>
@@ -7894,7 +8021,7 @@
       <c r="G127" s="46">
         <v>52</v>
       </c>
-      <c r="H127" s="158"/>
+      <c r="H127" s="169"/>
       <c r="I127" s="49">
         <f>G127*$H$126</f>
         <v>16.887128712871288</v>
@@ -7907,7 +8034,7 @@
       <c r="B128" s="46">
         <v>282</v>
       </c>
-      <c r="C128" s="158"/>
+      <c r="C128" s="169"/>
       <c r="D128" s="49">
         <f t="shared" si="2"/>
         <v>92.144656490470311</v>
@@ -7931,7 +8058,7 @@
       <c r="B129" s="46">
         <v>238</v>
       </c>
-      <c r="C129" s="158"/>
+      <c r="C129" s="169"/>
       <c r="D129" s="49">
         <f t="shared" si="2"/>
         <v>77.767476045148697</v>
@@ -7944,7 +8071,7 @@
       <c r="B130" s="46">
         <v>100</v>
       </c>
-      <c r="C130" s="158"/>
+      <c r="C130" s="169"/>
       <c r="D130" s="49">
         <f t="shared" si="2"/>
         <v>32.675410103003657</v>
@@ -7957,7 +8084,7 @@
       <c r="B131" s="46">
         <v>128</v>
       </c>
-      <c r="C131" s="158"/>
+      <c r="C131" s="169"/>
       <c r="D131" s="49">
         <f t="shared" si="2"/>
         <v>41.824524931844678</v>
@@ -7970,7 +8097,7 @@
       <c r="B132" s="46">
         <v>231</v>
       </c>
-      <c r="C132" s="158"/>
+      <c r="C132" s="169"/>
       <c r="D132" s="49">
         <f t="shared" si="2"/>
         <v>75.480197337938449</v>
@@ -7983,7 +8110,7 @@
       <c r="B133" s="46">
         <v>243</v>
       </c>
-      <c r="C133" s="158"/>
+      <c r="C133" s="169"/>
       <c r="D133" s="49">
         <f t="shared" si="2"/>
         <v>79.401246550298879</v>
@@ -7996,7 +8123,7 @@
       <c r="B134" s="46">
         <v>21</v>
       </c>
-      <c r="C134" s="158"/>
+      <c r="C134" s="169"/>
       <c r="D134" s="49">
         <f t="shared" si="2"/>
         <v>6.8618361216307679</v>
@@ -8009,7 +8136,7 @@
       <c r="B135" s="46">
         <v>126</v>
       </c>
-      <c r="C135" s="158"/>
+      <c r="C135" s="169"/>
       <c r="D135" s="49">
         <f t="shared" si="2"/>
         <v>41.171016729784604</v>
@@ -8047,11 +8174,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A117:A119"/>
-    <mergeCell ref="C126:C135"/>
-    <mergeCell ref="H126:H127"/>
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="B117:N117"/>
     <mergeCell ref="K2:K6"/>
     <mergeCell ref="A107:E107"/>
     <mergeCell ref="A108:E108"/>
@@ -8059,6 +8181,11 @@
     <mergeCell ref="F110:J110"/>
     <mergeCell ref="K8:K27"/>
     <mergeCell ref="K28:K40"/>
+    <mergeCell ref="A117:A119"/>
+    <mergeCell ref="C126:C135"/>
+    <mergeCell ref="H126:H127"/>
+    <mergeCell ref="B119:D119"/>
+    <mergeCell ref="B117:N117"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8071,8 +8198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9409B263-2852-4563-BF9F-9A2CBCD2EA0A}">
   <dimension ref="B2:S34"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -8288,27 +8415,27 @@
       </c>
     </row>
     <row r="12" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="181" t="s">
         <v>288</v>
       </c>
-      <c r="C12" s="165"/>
-      <c r="D12" s="165"/>
-      <c r="E12" s="165"/>
-      <c r="F12" s="165"/>
-      <c r="G12" s="165"/>
-      <c r="H12" s="165"/>
-      <c r="I12" s="165"/>
-      <c r="J12" s="165"/>
-      <c r="K12" s="165"/>
-      <c r="L12" s="165"/>
-      <c r="M12" s="165"/>
-      <c r="N12" s="165"/>
-      <c r="O12" s="165"/>
-      <c r="P12" s="165"/>
-      <c r="Q12" s="165"/>
+      <c r="C12" s="181"/>
+      <c r="D12" s="181"/>
+      <c r="E12" s="181"/>
+      <c r="F12" s="181"/>
+      <c r="G12" s="181"/>
+      <c r="H12" s="181"/>
+      <c r="I12" s="181"/>
+      <c r="J12" s="181"/>
+      <c r="K12" s="181"/>
+      <c r="L12" s="181"/>
+      <c r="M12" s="181"/>
+      <c r="N12" s="181"/>
+      <c r="O12" s="181"/>
+      <c r="P12" s="181"/>
+      <c r="Q12" s="181"/>
     </row>
     <row r="13" spans="2:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="166" t="s">
+      <c r="B13" s="182" t="s">
         <v>206</v>
       </c>
       <c r="C13" s="59">
@@ -8358,7 +8485,7 @@
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B14" s="167"/>
+      <c r="B14" s="183"/>
       <c r="C14" s="60">
         <f>SUM(C15:C22)</f>
         <v>57</v>
@@ -8835,23 +8962,23 @@
         <f t="shared" si="1"/>
         <v>2020</v>
       </c>
-      <c r="K28" s="225" t="s">
+      <c r="K28" s="188" t="s">
         <v>363</v>
       </c>
-      <c r="L28" s="226"/>
-      <c r="M28" s="226"/>
-      <c r="N28" s="226"/>
-      <c r="O28" s="227"/>
-      <c r="P28" s="217"/>
-      <c r="Q28" s="217"/>
-      <c r="R28" s="217"/>
-      <c r="S28" s="217"/>
+      <c r="L28" s="189"/>
+      <c r="M28" s="189"/>
+      <c r="N28" s="189"/>
+      <c r="O28" s="190"/>
+      <c r="P28" s="156"/>
+      <c r="Q28" s="156"/>
+      <c r="R28" s="156"/>
+      <c r="S28" s="156"/>
     </row>
     <row r="29" spans="2:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="231" t="s">
+      <c r="B29" s="184" t="s">
         <v>337</v>
       </c>
-      <c r="C29" s="232" t="s">
+      <c r="C29" s="165" t="s">
         <v>334</v>
       </c>
       <c r="D29" s="92">
@@ -8872,21 +8999,21 @@
       <c r="I29" s="92">
         <v>0</v>
       </c>
-      <c r="K29" s="219">
+      <c r="K29" s="158">
         <f>D30/D29</f>
         <v>0.75</v>
       </c>
-      <c r="L29" s="220"/>
-      <c r="M29" s="220"/>
-      <c r="N29" s="220"/>
-      <c r="O29" s="224">
+      <c r="L29" s="159"/>
+      <c r="M29" s="159"/>
+      <c r="N29" s="159"/>
+      <c r="O29" s="163">
         <f>AVERAGE(K29:N29)</f>
         <v>0.75</v>
       </c>
     </row>
     <row r="30" spans="2:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="233"/>
-      <c r="C30" s="232" t="s">
+      <c r="B30" s="185"/>
+      <c r="C30" s="165" t="s">
         <v>335</v>
       </c>
       <c r="D30" s="92">
@@ -8907,17 +9034,17 @@
       <c r="I30" s="92">
         <v>0</v>
       </c>
-      <c r="K30" s="219"/>
-      <c r="L30" s="220"/>
-      <c r="M30" s="220"/>
-      <c r="N30" s="220"/>
-      <c r="O30" s="221"/>
+      <c r="K30" s="158"/>
+      <c r="L30" s="159"/>
+      <c r="M30" s="159"/>
+      <c r="N30" s="159"/>
+      <c r="O30" s="160"/>
     </row>
     <row r="31" spans="2:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="228" t="s">
+      <c r="B31" s="186" t="s">
         <v>336</v>
       </c>
-      <c r="C31" s="229" t="s">
+      <c r="C31" s="164" t="s">
         <v>334</v>
       </c>
       <c r="D31" s="92">
@@ -8938,27 +9065,27 @@
       <c r="I31" s="92">
         <v>30</v>
       </c>
-      <c r="K31" s="222"/>
-      <c r="L31" s="223">
+      <c r="K31" s="161"/>
+      <c r="L31" s="162">
         <f t="shared" ref="L31" si="2">E32/E31</f>
         <v>0.8</v>
       </c>
-      <c r="M31" s="223">
+      <c r="M31" s="162">
         <f t="shared" ref="M31" si="3">F32/F31</f>
         <v>0.8666666666666667</v>
       </c>
-      <c r="N31" s="223">
+      <c r="N31" s="162">
         <f t="shared" ref="N31" si="4">G32/G31</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="O31" s="218">
+      <c r="O31" s="157">
         <f>AVERAGE(K31:N31)</f>
         <v>0.77777777777777779</v>
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="230"/>
-      <c r="C32" s="229" t="s">
+      <c r="B32" s="187"/>
+      <c r="C32" s="164" t="s">
         <v>335</v>
       </c>
       <c r="D32" s="92">
@@ -8981,59 +9108,59 @@
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C33" s="216" t="s">
+      <c r="C33" s="155" t="s">
         <v>361</v>
       </c>
-      <c r="D33" s="234">
+      <c r="D33" s="166">
         <f>+D29+D31</f>
         <v>20</v>
       </c>
-      <c r="E33" s="234">
+      <c r="E33" s="166">
         <f t="shared" ref="E33:I33" si="5">+E29+E31</f>
         <v>30</v>
       </c>
-      <c r="F33" s="234">
+      <c r="F33" s="166">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="G33" s="234">
+      <c r="G33" s="166">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="H33" s="234">
+      <c r="H33" s="166">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="I33" s="234">
+      <c r="I33" s="166">
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="216" t="s">
+      <c r="C34" s="155" t="s">
         <v>362</v>
       </c>
-      <c r="D34" s="235">
+      <c r="D34" s="167">
         <f>+D30+D32</f>
         <v>15</v>
       </c>
-      <c r="E34" s="235">
+      <c r="E34" s="167">
         <f t="shared" ref="E34:I34" si="6">+E30+E32</f>
         <v>24</v>
       </c>
-      <c r="F34" s="235">
+      <c r="F34" s="167">
         <f t="shared" si="6"/>
         <v>26</v>
       </c>
-      <c r="G34" s="235">
+      <c r="G34" s="167">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="H34" s="235">
+      <c r="H34" s="167">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="I34" s="235">
+      <c r="I34" s="167">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
@@ -9053,18 +9180,415 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE7CF57-8EE0-43FD-AF13-2469FC1B265B}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="236"/>
+    <col min="1" max="1" width="6" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="239" t="s">
+        <v>364</v>
+      </c>
+      <c r="C2" s="239"/>
+      <c r="D2" s="239"/>
+      <c r="E2" s="239"/>
+      <c r="F2" s="239"/>
+      <c r="G2" s="239"/>
+      <c r="H2" s="239"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="154" t="s">
+        <v>367</v>
+      </c>
+      <c r="C4" s="154">
+        <v>2005</v>
+      </c>
+      <c r="D4" s="154">
+        <f>+C4+1</f>
+        <v>2006</v>
+      </c>
+      <c r="E4" s="154">
+        <f t="shared" ref="E4:M4" si="0">+D4+1</f>
+        <v>2007</v>
+      </c>
+      <c r="F4" s="154">
+        <f t="shared" si="0"/>
+        <v>2008</v>
+      </c>
+      <c r="G4" s="154">
+        <f t="shared" si="0"/>
+        <v>2009</v>
+      </c>
+      <c r="H4" s="154">
+        <f t="shared" si="0"/>
+        <v>2010</v>
+      </c>
+      <c r="I4" s="154">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="J4" s="154">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="K4" s="154">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="L4" s="154">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="M4" s="154">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="241" t="s">
+        <v>365</v>
+      </c>
+      <c r="C5" s="153">
+        <f>+'Pobl. Ingresante Total'!C14</f>
+        <v>57</v>
+      </c>
+      <c r="D5" s="153">
+        <f>+'Pobl. Ingresante Total'!D14</f>
+        <v>47</v>
+      </c>
+      <c r="E5" s="153">
+        <f>+'Pobl. Ingresante Total'!E14</f>
+        <v>34</v>
+      </c>
+      <c r="F5" s="153">
+        <f>+'Pobl. Ingresante Total'!F14</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="153">
+        <f>+'Pobl. Ingresante Total'!G14</f>
+        <v>42</v>
+      </c>
+      <c r="H5" s="153">
+        <f>+'Pobl. Ingresante Total'!H14</f>
+        <v>41</v>
+      </c>
+      <c r="I5" s="153">
+        <f>+'Pobl. Ingresante Total'!I14</f>
+        <v>46</v>
+      </c>
+      <c r="J5" s="153">
+        <f>+'Pobl. Ingresante Total'!J14</f>
+        <v>40</v>
+      </c>
+      <c r="K5" s="153">
+        <f>+'Pobl. Ingresante Total'!K14</f>
+        <v>35</v>
+      </c>
+      <c r="L5" s="153">
+        <f>+'Pobl. Ingresante Total'!L14</f>
+        <v>37</v>
+      </c>
+      <c r="M5" s="153">
+        <f>+'matriculados Ind. Aprob.'!C11</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="240" t="s">
+        <v>369</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="152">
+        <f>(D5/C5)^(1/1)-1</f>
+        <v>-0.17543859649122806</v>
+      </c>
+      <c r="E6" s="152">
+        <f t="shared" ref="E6:M6" si="1">(E5/D5)^(1/1)-1</f>
+        <v>-0.27659574468085102</v>
+      </c>
+      <c r="F6" s="152"/>
+      <c r="G6" s="152">
+        <f>(G5/E5)^(1/2)-1</f>
+        <v>0.11143786045242265</v>
+      </c>
+      <c r="H6" s="152">
+        <f t="shared" si="1"/>
+        <v>-2.3809523809523836E-2</v>
+      </c>
+      <c r="I6" s="152">
+        <f t="shared" si="1"/>
+        <v>0.12195121951219523</v>
+      </c>
+      <c r="J6" s="152">
+        <f t="shared" si="1"/>
+        <v>-0.13043478260869568</v>
+      </c>
+      <c r="K6" s="152">
+        <f t="shared" si="1"/>
+        <v>-0.125</v>
+      </c>
+      <c r="L6" s="152">
+        <f t="shared" si="1"/>
+        <v>5.7142857142857162E-2</v>
+      </c>
+      <c r="M6" s="152">
+        <f t="shared" si="1"/>
+        <v>-8.108108108108103E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="242" t="s">
+        <v>366</v>
+      </c>
+      <c r="C7" s="246">
+        <f>(((D6+1)*(E6+1)*(F6+1)*(G6+1)*(H6+1)*(I6+1)*(J6+1)*(K6+1)*(L6+1)*(M6+1))^(1/9))-1</f>
+        <v>-6.6812820061970757E-2</v>
+      </c>
+      <c r="D7" s="247"/>
+      <c r="E7" s="247"/>
+      <c r="F7" s="247"/>
+      <c r="G7" s="247"/>
+      <c r="H7" s="247"/>
+      <c r="I7" s="247"/>
+      <c r="J7" s="247"/>
+      <c r="K7" s="247"/>
+      <c r="L7" s="248"/>
+      <c r="M7" s="45"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="154" t="s">
+        <v>367</v>
+      </c>
+      <c r="C10" s="154">
+        <v>2015</v>
+      </c>
+      <c r="D10" s="154">
+        <f>+C10+1</f>
+        <v>2016</v>
+      </c>
+      <c r="E10" s="154">
+        <f t="shared" ref="E10:J10" si="2">+D10+1</f>
+        <v>2017</v>
+      </c>
+      <c r="F10" s="154">
+        <f t="shared" si="2"/>
+        <v>2018</v>
+      </c>
+      <c r="G10" s="154">
+        <f t="shared" si="2"/>
+        <v>2019</v>
+      </c>
+      <c r="H10" s="154">
+        <f t="shared" si="2"/>
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="243" t="s">
+        <v>365</v>
+      </c>
+      <c r="C11" s="153">
+        <f>+'Pobl. Ingresante Total'!M14</f>
+        <v>33</v>
+      </c>
+      <c r="D11" s="153">
+        <f>+'Pobl. Ingresante Total'!N14</f>
+        <v>39</v>
+      </c>
+      <c r="E11" s="153">
+        <f>+'Pobl. Ingresante Total'!O14</f>
+        <v>50</v>
+      </c>
+      <c r="F11" s="153">
+        <f>+'Pobl. Ingresante Total'!P14</f>
+        <v>61</v>
+      </c>
+      <c r="G11" s="153">
+        <f>+'Pobl. Ingresante Total'!Q14</f>
+        <v>50</v>
+      </c>
+      <c r="H11" s="153">
+        <f>+'matriculados Ind. Aprob.'!M33</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B12" s="244" t="s">
+        <v>368</v>
+      </c>
+      <c r="C12" s="45"/>
+      <c r="D12" s="152">
+        <f>(D11/C11)^(1/1)-1</f>
+        <v>0.18181818181818188</v>
+      </c>
+      <c r="E12" s="152">
+        <f t="shared" ref="E12:H12" si="3">(E11/D11)^(1/1)-1</f>
+        <v>0.28205128205128216</v>
+      </c>
+      <c r="F12" s="152">
+        <f t="shared" si="3"/>
+        <v>0.21999999999999997</v>
+      </c>
+      <c r="G12" s="152">
+        <f t="shared" si="3"/>
+        <v>-0.18032786885245899</v>
+      </c>
+      <c r="H12" s="152">
+        <f t="shared" si="3"/>
+        <v>0.10000000000000009</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="245" t="s">
+        <v>366</v>
+      </c>
+      <c r="C13" s="169">
+        <f>(((D12+1)*(E12+1)*(F12+1)*(G12+1)*(H12+1))^(1/4))-1</f>
+        <v>0.13621936646749933</v>
+      </c>
+      <c r="D13" s="169"/>
+      <c r="E13" s="169"/>
+      <c r="F13" s="169"/>
+      <c r="G13" s="169"/>
+      <c r="H13" s="169"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="252" t="s">
+        <v>371</v>
+      </c>
+      <c r="C18" s="250" t="s">
+        <v>373</v>
+      </c>
+      <c r="D18" s="249"/>
+      <c r="E18" s="154" t="s">
+        <v>374</v>
+      </c>
+      <c r="F18" s="154" t="s">
+        <v>375</v>
+      </c>
+      <c r="G18" s="154" t="s">
+        <v>376</v>
+      </c>
+      <c r="H18" s="154" t="s">
+        <v>377</v>
+      </c>
+      <c r="I18" s="154" t="s">
+        <v>378</v>
+      </c>
+      <c r="J18" s="154" t="s">
+        <v>379</v>
+      </c>
+      <c r="K18" s="154" t="s">
+        <v>380</v>
+      </c>
+      <c r="L18" s="154" t="s">
+        <v>381</v>
+      </c>
+      <c r="M18" s="154" t="s">
+        <v>382</v>
+      </c>
+      <c r="N18" s="154" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="252"/>
+      <c r="C19" s="251">
+        <v>2020</v>
+      </c>
+      <c r="D19" s="154">
+        <f>+C19+1</f>
+        <v>2021</v>
+      </c>
+      <c r="E19" s="154">
+        <f t="shared" ref="E19:N19" si="4">+D19+1</f>
+        <v>2022</v>
+      </c>
+      <c r="F19" s="154">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="G19" s="154">
+        <f t="shared" si="4"/>
+        <v>2024</v>
+      </c>
+      <c r="H19" s="154">
+        <f t="shared" si="4"/>
+        <v>2025</v>
+      </c>
+      <c r="I19" s="154">
+        <f t="shared" si="4"/>
+        <v>2026</v>
+      </c>
+      <c r="J19" s="154">
+        <f t="shared" si="4"/>
+        <v>2027</v>
+      </c>
+      <c r="K19" s="154">
+        <f t="shared" si="4"/>
+        <v>2028</v>
+      </c>
+      <c r="L19" s="154">
+        <f t="shared" si="4"/>
+        <v>2029</v>
+      </c>
+      <c r="M19" s="154">
+        <f t="shared" si="4"/>
+        <v>2030</v>
+      </c>
+      <c r="N19" s="154">
+        <f t="shared" si="4"/>
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="89" t="s">
+        <v>372</v>
+      </c>
+      <c r="C20" s="153"/>
+      <c r="D20" s="153"/>
+      <c r="E20" s="153"/>
+      <c r="F20" s="153"/>
+      <c r="G20" s="153"/>
+      <c r="H20" s="153"/>
+      <c r="I20" s="153"/>
+      <c r="J20" s="153"/>
+      <c r="K20" s="153"/>
+      <c r="L20" s="153"/>
+      <c r="M20" s="153"/>
+      <c r="N20" s="153"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C7:L7"/>
+    <mergeCell ref="C13:H13"/>
+  </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9095,69 +9619,69 @@
   <sheetData>
     <row r="1" spans="1:51" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:51" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="V2" s="211" t="s">
+      <c r="V2" s="191" t="s">
         <v>338</v>
       </c>
-      <c r="W2" s="212"/>
-      <c r="X2" s="212"/>
-      <c r="Y2" s="212"/>
-      <c r="Z2" s="212"/>
-      <c r="AA2" s="212"/>
-      <c r="AB2" s="212"/>
-      <c r="AC2" s="212"/>
-      <c r="AD2" s="212"/>
-      <c r="AE2" s="212"/>
-      <c r="AF2" s="212"/>
-      <c r="AG2" s="212"/>
-      <c r="AH2" s="212"/>
-      <c r="AI2" s="212"/>
-      <c r="AJ2" s="212"/>
-      <c r="AK2" s="212"/>
-      <c r="AL2" s="212"/>
-      <c r="AM2" s="212"/>
-      <c r="AN2" s="212"/>
-      <c r="AO2" s="212"/>
-      <c r="AP2" s="212"/>
-      <c r="AQ2" s="212"/>
-      <c r="AR2" s="212"/>
-      <c r="AS2" s="213"/>
+      <c r="W2" s="192"/>
+      <c r="X2" s="192"/>
+      <c r="Y2" s="192"/>
+      <c r="Z2" s="192"/>
+      <c r="AA2" s="192"/>
+      <c r="AB2" s="192"/>
+      <c r="AC2" s="192"/>
+      <c r="AD2" s="192"/>
+      <c r="AE2" s="192"/>
+      <c r="AF2" s="192"/>
+      <c r="AG2" s="192"/>
+      <c r="AH2" s="192"/>
+      <c r="AI2" s="192"/>
+      <c r="AJ2" s="192"/>
+      <c r="AK2" s="192"/>
+      <c r="AL2" s="192"/>
+      <c r="AM2" s="192"/>
+      <c r="AN2" s="192"/>
+      <c r="AO2" s="192"/>
+      <c r="AP2" s="192"/>
+      <c r="AQ2" s="192"/>
+      <c r="AR2" s="192"/>
+      <c r="AS2" s="193"/>
       <c r="AT2" s="83"/>
       <c r="AU2" s="83"/>
     </row>
     <row r="3" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A3" s="214" t="s">
+      <c r="A3" s="194" t="s">
         <v>349</v>
       </c>
-      <c r="B3" s="214"/>
-      <c r="C3" s="168">
+      <c r="B3" s="194"/>
+      <c r="C3" s="195">
         <v>2015</v>
       </c>
-      <c r="D3" s="168"/>
-      <c r="E3" s="168">
+      <c r="D3" s="195"/>
+      <c r="E3" s="195">
         <f>+C3+1</f>
         <v>2016</v>
       </c>
-      <c r="F3" s="168"/>
-      <c r="G3" s="168">
+      <c r="F3" s="195"/>
+      <c r="G3" s="195">
         <f t="shared" ref="G3" si="0">+E3+1</f>
         <v>2017</v>
       </c>
-      <c r="H3" s="168"/>
-      <c r="I3" s="168">
+      <c r="H3" s="195"/>
+      <c r="I3" s="195">
         <f t="shared" ref="I3" si="1">+G3+1</f>
         <v>2018</v>
       </c>
-      <c r="J3" s="168"/>
-      <c r="K3" s="168">
+      <c r="J3" s="195"/>
+      <c r="K3" s="195">
         <f t="shared" ref="K3" si="2">+I3+1</f>
         <v>2019</v>
       </c>
-      <c r="L3" s="168"/>
-      <c r="M3" s="168">
+      <c r="L3" s="195"/>
+      <c r="M3" s="195">
         <f t="shared" ref="M3" si="3">+K3+1</f>
         <v>2020</v>
       </c>
-      <c r="N3" s="168"/>
+      <c r="N3" s="195"/>
       <c r="P3" s="136" t="s">
         <v>355</v>
       </c>
@@ -9167,74 +9691,74 @@
       <c r="T3" s="84" t="s">
         <v>356</v>
       </c>
-      <c r="V3" s="215">
+      <c r="V3" s="196">
         <v>2020</v>
       </c>
-      <c r="W3" s="203"/>
-      <c r="X3" s="203">
+      <c r="W3" s="197"/>
+      <c r="X3" s="197">
         <f>+V3+1</f>
         <v>2021</v>
       </c>
-      <c r="Y3" s="203"/>
-      <c r="Z3" s="203">
+      <c r="Y3" s="197"/>
+      <c r="Z3" s="197">
         <f t="shared" ref="Z3" si="4">+X3+1</f>
         <v>2022</v>
       </c>
-      <c r="AA3" s="203"/>
-      <c r="AB3" s="203">
+      <c r="AA3" s="197"/>
+      <c r="AB3" s="197">
         <f t="shared" ref="AB3" si="5">+Z3+1</f>
         <v>2023</v>
       </c>
-      <c r="AC3" s="203"/>
-      <c r="AD3" s="203">
+      <c r="AC3" s="197"/>
+      <c r="AD3" s="197">
         <f t="shared" ref="AD3" si="6">+AB3+1</f>
         <v>2024</v>
       </c>
-      <c r="AE3" s="203"/>
-      <c r="AF3" s="203">
+      <c r="AE3" s="197"/>
+      <c r="AF3" s="197">
         <f t="shared" ref="AF3" si="7">+AD3+1</f>
         <v>2025</v>
       </c>
-      <c r="AG3" s="203"/>
-      <c r="AH3" s="203">
+      <c r="AG3" s="197"/>
+      <c r="AH3" s="197">
         <f t="shared" ref="AH3" si="8">+AF3+1</f>
         <v>2026</v>
       </c>
-      <c r="AI3" s="203"/>
-      <c r="AJ3" s="203">
+      <c r="AI3" s="197"/>
+      <c r="AJ3" s="197">
         <f t="shared" ref="AJ3" si="9">+AH3+1</f>
         <v>2027</v>
       </c>
-      <c r="AK3" s="203"/>
-      <c r="AL3" s="203">
+      <c r="AK3" s="197"/>
+      <c r="AL3" s="197">
         <f t="shared" ref="AL3" si="10">+AJ3+1</f>
         <v>2028</v>
       </c>
-      <c r="AM3" s="203"/>
-      <c r="AN3" s="203">
+      <c r="AM3" s="197"/>
+      <c r="AN3" s="197">
         <f t="shared" ref="AN3" si="11">+AL3+1</f>
         <v>2029</v>
       </c>
-      <c r="AO3" s="203"/>
-      <c r="AP3" s="203">
+      <c r="AO3" s="197"/>
+      <c r="AP3" s="197">
         <f t="shared" ref="AP3" si="12">+AN3+1</f>
         <v>2030</v>
       </c>
-      <c r="AQ3" s="203"/>
-      <c r="AR3" s="203">
+      <c r="AQ3" s="197"/>
+      <c r="AR3" s="197">
         <f t="shared" ref="AR3" si="13">+AP3+1</f>
         <v>2031</v>
       </c>
-      <c r="AS3" s="204"/>
-      <c r="AT3" s="205">
+      <c r="AS3" s="198"/>
+      <c r="AT3" s="199">
         <f t="shared" ref="AT3" si="14">+AR3+1</f>
         <v>2032</v>
       </c>
-      <c r="AU3" s="206"/>
+      <c r="AU3" s="200"/>
     </row>
     <row r="4" spans="1:51" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="214"/>
-      <c r="B4" s="214"/>
+      <c r="A4" s="194"/>
+      <c r="B4" s="194"/>
       <c r="C4" s="115" t="s">
         <v>280</v>
       </c>
@@ -9362,7 +9886,7 @@
       </c>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A5" s="207" t="s">
+      <c r="A5" s="201" t="s">
         <v>339</v>
       </c>
       <c r="B5" s="32" t="s">
@@ -9428,7 +9952,7 @@
       <c r="AU5" s="146"/>
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A6" s="207"/>
+      <c r="A6" s="201"/>
       <c r="B6" s="32" t="s">
         <v>281</v>
       </c>
@@ -9492,7 +10016,7 @@
       </c>
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A7" s="207"/>
+      <c r="A7" s="201"/>
       <c r="B7" s="32" t="s">
         <v>282</v>
       </c>
@@ -9555,7 +10079,7 @@
       <c r="AU7" s="146"/>
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A8" s="207"/>
+      <c r="A8" s="201"/>
       <c r="B8" s="32" t="s">
         <v>283</v>
       </c>
@@ -9618,7 +10142,7 @@
       <c r="AU8" s="146"/>
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.25">
-      <c r="A9" s="207"/>
+      <c r="A9" s="201"/>
       <c r="B9" s="32" t="s">
         <v>284</v>
       </c>
@@ -9683,7 +10207,7 @@
       <c r="AU9" s="146"/>
     </row>
     <row r="10" spans="1:51" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="207"/>
+      <c r="A10" s="201"/>
       <c r="B10" s="32" t="s">
         <v>285</v>
       </c>
@@ -9748,7 +10272,7 @@
       <c r="AU10" s="146"/>
     </row>
     <row r="11" spans="1:51" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="207"/>
+      <c r="A11" s="201"/>
       <c r="B11" s="32" t="s">
         <v>340</v>
       </c>
@@ -9840,124 +10364,124 @@
     </row>
     <row r="12" spans="1:51" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:51" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="V13" s="208" t="s">
+      <c r="V13" s="202" t="s">
         <v>341</v>
       </c>
-      <c r="W13" s="209"/>
-      <c r="X13" s="209"/>
-      <c r="Y13" s="209"/>
-      <c r="Z13" s="209"/>
-      <c r="AA13" s="209"/>
-      <c r="AB13" s="209"/>
-      <c r="AC13" s="209"/>
-      <c r="AD13" s="209"/>
-      <c r="AE13" s="209"/>
-      <c r="AF13" s="209"/>
-      <c r="AG13" s="209"/>
-      <c r="AH13" s="209"/>
-      <c r="AI13" s="209"/>
-      <c r="AJ13" s="209"/>
-      <c r="AK13" s="209"/>
-      <c r="AL13" s="209"/>
-      <c r="AM13" s="209"/>
-      <c r="AN13" s="209"/>
-      <c r="AO13" s="209"/>
-      <c r="AP13" s="209"/>
-      <c r="AQ13" s="209"/>
-      <c r="AR13" s="209"/>
-      <c r="AS13" s="209"/>
-      <c r="AT13" s="209"/>
-      <c r="AU13" s="210"/>
+      <c r="W13" s="203"/>
+      <c r="X13" s="203"/>
+      <c r="Y13" s="203"/>
+      <c r="Z13" s="203"/>
+      <c r="AA13" s="203"/>
+      <c r="AB13" s="203"/>
+      <c r="AC13" s="203"/>
+      <c r="AD13" s="203"/>
+      <c r="AE13" s="203"/>
+      <c r="AF13" s="203"/>
+      <c r="AG13" s="203"/>
+      <c r="AH13" s="203"/>
+      <c r="AI13" s="203"/>
+      <c r="AJ13" s="203"/>
+      <c r="AK13" s="203"/>
+      <c r="AL13" s="203"/>
+      <c r="AM13" s="203"/>
+      <c r="AN13" s="203"/>
+      <c r="AO13" s="203"/>
+      <c r="AP13" s="203"/>
+      <c r="AQ13" s="203"/>
+      <c r="AR13" s="203"/>
+      <c r="AS13" s="203"/>
+      <c r="AT13" s="203"/>
+      <c r="AU13" s="204"/>
     </row>
     <row r="14" spans="1:51" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="195" t="s">
+      <c r="A14" s="215" t="s">
         <v>342</v>
       </c>
-      <c r="B14" s="196" t="s">
+      <c r="B14" s="216" t="s">
         <v>343</v>
       </c>
-      <c r="C14" s="197"/>
-      <c r="D14" s="200" t="s">
+      <c r="C14" s="217"/>
+      <c r="D14" s="220" t="s">
         <v>344</v>
       </c>
-      <c r="E14" s="201"/>
-      <c r="F14" s="200"/>
-      <c r="G14" s="201"/>
-      <c r="H14" s="200"/>
-      <c r="I14" s="201"/>
+      <c r="E14" s="221"/>
+      <c r="F14" s="220"/>
+      <c r="G14" s="221"/>
+      <c r="H14" s="220"/>
+      <c r="I14" s="221"/>
       <c r="K14" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="V14" s="202">
+      <c r="V14" s="222">
         <f>+V3</f>
         <v>2020</v>
       </c>
-      <c r="W14" s="193"/>
-      <c r="X14" s="193">
+      <c r="W14" s="207"/>
+      <c r="X14" s="207">
         <f>+V14+1</f>
         <v>2021</v>
       </c>
-      <c r="Y14" s="193"/>
-      <c r="Z14" s="193">
+      <c r="Y14" s="207"/>
+      <c r="Z14" s="207">
         <f t="shared" ref="Z14" si="17">+X14+1</f>
         <v>2022</v>
       </c>
-      <c r="AA14" s="193"/>
-      <c r="AB14" s="193">
+      <c r="AA14" s="207"/>
+      <c r="AB14" s="207">
         <f t="shared" ref="AB14" si="18">+Z14+1</f>
         <v>2023</v>
       </c>
-      <c r="AC14" s="193"/>
-      <c r="AD14" s="193">
+      <c r="AC14" s="207"/>
+      <c r="AD14" s="207">
         <f t="shared" ref="AD14" si="19">+AB14+1</f>
         <v>2024</v>
       </c>
-      <c r="AE14" s="193"/>
-      <c r="AF14" s="193">
+      <c r="AE14" s="207"/>
+      <c r="AF14" s="207">
         <f t="shared" ref="AF14" si="20">+AD14+1</f>
         <v>2025</v>
       </c>
-      <c r="AG14" s="193"/>
-      <c r="AH14" s="193">
+      <c r="AG14" s="207"/>
+      <c r="AH14" s="207">
         <f t="shared" ref="AH14" si="21">+AF14+1</f>
         <v>2026</v>
       </c>
-      <c r="AI14" s="193"/>
-      <c r="AJ14" s="193">
+      <c r="AI14" s="207"/>
+      <c r="AJ14" s="207">
         <f t="shared" ref="AJ14" si="22">+AH14+1</f>
         <v>2027</v>
       </c>
-      <c r="AK14" s="193"/>
-      <c r="AL14" s="193">
+      <c r="AK14" s="207"/>
+      <c r="AL14" s="207">
         <f t="shared" ref="AL14" si="23">+AJ14+1</f>
         <v>2028</v>
       </c>
-      <c r="AM14" s="193"/>
-      <c r="AN14" s="193">
+      <c r="AM14" s="207"/>
+      <c r="AN14" s="207">
         <f t="shared" ref="AN14" si="24">+AL14+1</f>
         <v>2029</v>
       </c>
-      <c r="AO14" s="193"/>
-      <c r="AP14" s="193">
+      <c r="AO14" s="207"/>
+      <c r="AP14" s="207">
         <f t="shared" ref="AP14" si="25">+AN14+1</f>
         <v>2030</v>
       </c>
-      <c r="AQ14" s="193"/>
-      <c r="AR14" s="193">
+      <c r="AQ14" s="207"/>
+      <c r="AR14" s="207">
         <f t="shared" ref="AR14" si="26">+AP14+1</f>
         <v>2031</v>
       </c>
-      <c r="AS14" s="193"/>
-      <c r="AT14" s="193">
+      <c r="AS14" s="207"/>
+      <c r="AT14" s="207">
         <f t="shared" ref="AT14" si="27">+AR14+1</f>
         <v>2032</v>
       </c>
-      <c r="AU14" s="194"/>
+      <c r="AU14" s="208"/>
     </row>
     <row r="15" spans="1:51" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="195"/>
-      <c r="B15" s="198"/>
-      <c r="C15" s="199"/>
+      <c r="A15" s="215"/>
+      <c r="B15" s="218"/>
+      <c r="C15" s="219"/>
       <c r="D15" s="102" t="s">
         <v>346</v>
       </c>
@@ -10048,11 +10572,11 @@
       </c>
     </row>
     <row r="16" spans="1:51" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="195"/>
-      <c r="B16" s="174" t="s">
+      <c r="A16" s="215"/>
+      <c r="B16" s="205" t="s">
         <v>280</v>
       </c>
-      <c r="C16" s="175"/>
+      <c r="C16" s="206"/>
       <c r="D16" s="93"/>
       <c r="E16" s="94"/>
       <c r="F16" s="93"/>
@@ -10105,11 +10629,11 @@
       <c r="AU16" s="146"/>
     </row>
     <row r="17" spans="1:47" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="195"/>
-      <c r="B17" s="174" t="s">
+      <c r="A17" s="215"/>
+      <c r="B17" s="205" t="s">
         <v>281</v>
       </c>
-      <c r="C17" s="175"/>
+      <c r="C17" s="206"/>
       <c r="D17" s="118">
         <f>+D6/C5</f>
         <v>0.73333333333333328</v>
@@ -10176,11 +10700,11 @@
       </c>
     </row>
     <row r="18" spans="1:47" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="195"/>
-      <c r="B18" s="174" t="s">
+      <c r="A18" s="215"/>
+      <c r="B18" s="205" t="s">
         <v>282</v>
       </c>
-      <c r="C18" s="175"/>
+      <c r="C18" s="206"/>
       <c r="D18" s="118">
         <f>+E7/C5</f>
         <v>0.53333333333333333</v>
@@ -10244,11 +10768,11 @@
       <c r="AU18" s="146"/>
     </row>
     <row r="19" spans="1:47" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="195"/>
-      <c r="B19" s="174" t="s">
+      <c r="A19" s="215"/>
+      <c r="B19" s="205" t="s">
         <v>283</v>
       </c>
-      <c r="C19" s="175"/>
+      <c r="C19" s="206"/>
       <c r="D19" s="120">
         <f>+F8/C5</f>
         <v>0.53333333333333333</v>
@@ -10312,11 +10836,11 @@
       <c r="AU19" s="146"/>
     </row>
     <row r="20" spans="1:47" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="195"/>
-      <c r="B20" s="174" t="s">
+      <c r="A20" s="215"/>
+      <c r="B20" s="205" t="s">
         <v>284</v>
       </c>
-      <c r="C20" s="175"/>
+      <c r="C20" s="206"/>
       <c r="D20" s="120">
         <f>+G9/C5</f>
         <v>0.26666666666666666</v>
@@ -10380,11 +10904,11 @@
       <c r="AU20" s="146"/>
     </row>
     <row r="21" spans="1:47" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="195"/>
-      <c r="B21" s="174" t="s">
+      <c r="A21" s="215"/>
+      <c r="B21" s="205" t="s">
         <v>285</v>
       </c>
-      <c r="C21" s="175"/>
+      <c r="C21" s="206"/>
       <c r="D21" s="121">
         <f>+H10/C5</f>
         <v>0.26666666666666666</v>
@@ -10486,72 +11010,72 @@
       </c>
     </row>
     <row r="25" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A25" s="191" t="s">
+      <c r="A25" s="212" t="s">
         <v>348</v>
       </c>
-      <c r="B25" s="191"/>
-      <c r="C25" s="169">
+      <c r="B25" s="212"/>
+      <c r="C25" s="213">
         <f>+C3</f>
         <v>2015</v>
       </c>
-      <c r="D25" s="169"/>
-      <c r="E25" s="169">
+      <c r="D25" s="213"/>
+      <c r="E25" s="213">
         <f>+C25+1</f>
         <v>2016</v>
       </c>
-      <c r="F25" s="169"/>
-      <c r="G25" s="169">
+      <c r="F25" s="213"/>
+      <c r="G25" s="213">
         <f t="shared" ref="G25" si="29">+E25+1</f>
         <v>2017</v>
       </c>
-      <c r="H25" s="169"/>
-      <c r="I25" s="169">
+      <c r="H25" s="213"/>
+      <c r="I25" s="213">
         <f t="shared" ref="I25" si="30">+G25+1</f>
         <v>2018</v>
       </c>
-      <c r="J25" s="169"/>
-      <c r="K25" s="169">
+      <c r="J25" s="213"/>
+      <c r="K25" s="213">
         <f t="shared" ref="K25" si="31">+I25+1</f>
         <v>2019</v>
       </c>
-      <c r="L25" s="169"/>
-      <c r="M25" s="169">
+      <c r="L25" s="213"/>
+      <c r="M25" s="213">
         <f t="shared" ref="M25" si="32">+K25+1</f>
         <v>2020</v>
       </c>
-      <c r="N25" s="169"/>
-      <c r="V25" s="188" t="s">
+      <c r="N25" s="213"/>
+      <c r="V25" s="209" t="s">
         <v>338</v>
       </c>
-      <c r="W25" s="189"/>
-      <c r="X25" s="189"/>
-      <c r="Y25" s="189"/>
-      <c r="Z25" s="189"/>
-      <c r="AA25" s="189"/>
-      <c r="AB25" s="189"/>
-      <c r="AC25" s="189"/>
-      <c r="AD25" s="189"/>
-      <c r="AE25" s="189"/>
-      <c r="AF25" s="189"/>
-      <c r="AG25" s="189"/>
-      <c r="AH25" s="189"/>
-      <c r="AI25" s="189"/>
-      <c r="AJ25" s="189"/>
-      <c r="AK25" s="189"/>
-      <c r="AL25" s="189"/>
-      <c r="AM25" s="189"/>
-      <c r="AN25" s="189"/>
-      <c r="AO25" s="189"/>
-      <c r="AP25" s="189"/>
-      <c r="AQ25" s="189"/>
-      <c r="AR25" s="189"/>
-      <c r="AS25" s="189"/>
-      <c r="AT25" s="189"/>
-      <c r="AU25" s="190"/>
+      <c r="W25" s="210"/>
+      <c r="X25" s="210"/>
+      <c r="Y25" s="210"/>
+      <c r="Z25" s="210"/>
+      <c r="AA25" s="210"/>
+      <c r="AB25" s="210"/>
+      <c r="AC25" s="210"/>
+      <c r="AD25" s="210"/>
+      <c r="AE25" s="210"/>
+      <c r="AF25" s="210"/>
+      <c r="AG25" s="210"/>
+      <c r="AH25" s="210"/>
+      <c r="AI25" s="210"/>
+      <c r="AJ25" s="210"/>
+      <c r="AK25" s="210"/>
+      <c r="AL25" s="210"/>
+      <c r="AM25" s="210"/>
+      <c r="AN25" s="210"/>
+      <c r="AO25" s="210"/>
+      <c r="AP25" s="210"/>
+      <c r="AQ25" s="210"/>
+      <c r="AR25" s="210"/>
+      <c r="AS25" s="210"/>
+      <c r="AT25" s="210"/>
+      <c r="AU25" s="211"/>
     </row>
     <row r="26" spans="1:47" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="191"/>
-      <c r="B26" s="191"/>
+      <c r="A26" s="212"/>
+      <c r="B26" s="212"/>
       <c r="C26" s="98" t="s">
         <v>280</v>
       </c>
@@ -10603,74 +11127,74 @@
       <c r="T26" s="97" t="s">
         <v>356</v>
       </c>
-      <c r="V26" s="192">
+      <c r="V26" s="214">
         <f>+V3</f>
         <v>2020</v>
       </c>
-      <c r="W26" s="169"/>
-      <c r="X26" s="169">
+      <c r="W26" s="213"/>
+      <c r="X26" s="213">
         <f>+V26+1</f>
         <v>2021</v>
       </c>
-      <c r="Y26" s="169"/>
-      <c r="Z26" s="169">
+      <c r="Y26" s="213"/>
+      <c r="Z26" s="213">
         <f t="shared" ref="Z26" si="33">+X26+1</f>
         <v>2022</v>
       </c>
-      <c r="AA26" s="169"/>
-      <c r="AB26" s="169">
+      <c r="AA26" s="213"/>
+      <c r="AB26" s="213">
         <f t="shared" ref="AB26" si="34">+Z26+1</f>
         <v>2023</v>
       </c>
-      <c r="AC26" s="169"/>
-      <c r="AD26" s="169">
+      <c r="AC26" s="213"/>
+      <c r="AD26" s="213">
         <f t="shared" ref="AD26" si="35">+AB26+1</f>
         <v>2024</v>
       </c>
-      <c r="AE26" s="169"/>
-      <c r="AF26" s="169">
+      <c r="AE26" s="213"/>
+      <c r="AF26" s="213">
         <f t="shared" ref="AF26" si="36">+AD26+1</f>
         <v>2025</v>
       </c>
-      <c r="AG26" s="169"/>
-      <c r="AH26" s="169">
+      <c r="AG26" s="213"/>
+      <c r="AH26" s="213">
         <f t="shared" ref="AH26" si="37">+AF26+1</f>
         <v>2026</v>
       </c>
-      <c r="AI26" s="169"/>
-      <c r="AJ26" s="169">
+      <c r="AI26" s="213"/>
+      <c r="AJ26" s="213">
         <f t="shared" ref="AJ26" si="38">+AH26+1</f>
         <v>2027</v>
       </c>
-      <c r="AK26" s="169"/>
-      <c r="AL26" s="169">
+      <c r="AK26" s="213"/>
+      <c r="AL26" s="213">
         <f t="shared" ref="AL26" si="39">+AJ26+1</f>
         <v>2028</v>
       </c>
-      <c r="AM26" s="169"/>
-      <c r="AN26" s="169">
+      <c r="AM26" s="213"/>
+      <c r="AN26" s="213">
         <f t="shared" ref="AN26" si="40">+AL26+1</f>
         <v>2029</v>
       </c>
-      <c r="AO26" s="169"/>
-      <c r="AP26" s="169">
+      <c r="AO26" s="213"/>
+      <c r="AP26" s="213">
         <f t="shared" ref="AP26" si="41">+AN26+1</f>
         <v>2030</v>
       </c>
-      <c r="AQ26" s="169"/>
-      <c r="AR26" s="169">
+      <c r="AQ26" s="213"/>
+      <c r="AR26" s="213">
         <f t="shared" ref="AR26" si="42">+AP26+1</f>
         <v>2031</v>
       </c>
-      <c r="AS26" s="169"/>
-      <c r="AT26" s="169">
+      <c r="AS26" s="213"/>
+      <c r="AT26" s="213">
         <f t="shared" ref="AT26" si="43">+AR26+1</f>
         <v>2032</v>
       </c>
-      <c r="AU26" s="187"/>
+      <c r="AU26" s="223"/>
     </row>
     <row r="27" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A27" s="169" t="s">
+      <c r="A27" s="213" t="s">
         <v>339</v>
       </c>
       <c r="B27" s="99" t="s">
@@ -10798,7 +11322,7 @@
       </c>
     </row>
     <row r="28" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A28" s="169"/>
+      <c r="A28" s="213"/>
       <c r="B28" s="99" t="s">
         <v>281</v>
       </c>
@@ -10892,7 +11416,7 @@
       <c r="AU28" s="105"/>
     </row>
     <row r="29" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A29" s="169"/>
+      <c r="A29" s="213"/>
       <c r="B29" s="99" t="s">
         <v>282</v>
       </c>
@@ -10986,7 +11510,7 @@
       </c>
     </row>
     <row r="30" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A30" s="169"/>
+      <c r="A30" s="213"/>
       <c r="B30" s="99" t="s">
         <v>283</v>
       </c>
@@ -11075,7 +11599,7 @@
       <c r="AU30" s="105"/>
     </row>
     <row r="31" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A31" s="169"/>
+      <c r="A31" s="213"/>
       <c r="B31" s="99" t="s">
         <v>284</v>
       </c>
@@ -11164,7 +11688,7 @@
       </c>
     </row>
     <row r="32" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A32" s="169"/>
+      <c r="A32" s="213"/>
       <c r="B32" s="99" t="s">
         <v>285</v>
       </c>
@@ -11248,7 +11772,7 @@
       <c r="AU32" s="105"/>
     </row>
     <row r="33" spans="1:47" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="169"/>
+      <c r="A33" s="213"/>
       <c r="B33" s="99" t="s">
         <v>340</v>
       </c>
@@ -11365,137 +11889,137 @@
     </row>
     <row r="34" spans="1:47" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:47" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="V35" s="178" t="s">
+      <c r="V35" s="224" t="s">
         <v>341</v>
       </c>
-      <c r="W35" s="179"/>
-      <c r="X35" s="179"/>
-      <c r="Y35" s="179"/>
-      <c r="Z35" s="179"/>
-      <c r="AA35" s="179"/>
-      <c r="AB35" s="179"/>
-      <c r="AC35" s="179"/>
-      <c r="AD35" s="179"/>
-      <c r="AE35" s="179"/>
-      <c r="AF35" s="179"/>
-      <c r="AG35" s="179"/>
-      <c r="AH35" s="179"/>
-      <c r="AI35" s="179"/>
-      <c r="AJ35" s="179"/>
-      <c r="AK35" s="179"/>
-      <c r="AL35" s="179"/>
-      <c r="AM35" s="179"/>
-      <c r="AN35" s="179"/>
-      <c r="AO35" s="179"/>
-      <c r="AP35" s="179"/>
-      <c r="AQ35" s="179"/>
-      <c r="AR35" s="179"/>
-      <c r="AS35" s="179"/>
-      <c r="AT35" s="179"/>
-      <c r="AU35" s="180"/>
+      <c r="W35" s="225"/>
+      <c r="X35" s="225"/>
+      <c r="Y35" s="225"/>
+      <c r="Z35" s="225"/>
+      <c r="AA35" s="225"/>
+      <c r="AB35" s="225"/>
+      <c r="AC35" s="225"/>
+      <c r="AD35" s="225"/>
+      <c r="AE35" s="225"/>
+      <c r="AF35" s="225"/>
+      <c r="AG35" s="225"/>
+      <c r="AH35" s="225"/>
+      <c r="AI35" s="225"/>
+      <c r="AJ35" s="225"/>
+      <c r="AK35" s="225"/>
+      <c r="AL35" s="225"/>
+      <c r="AM35" s="225"/>
+      <c r="AN35" s="225"/>
+      <c r="AO35" s="225"/>
+      <c r="AP35" s="225"/>
+      <c r="AQ35" s="225"/>
+      <c r="AR35" s="225"/>
+      <c r="AS35" s="225"/>
+      <c r="AT35" s="225"/>
+      <c r="AU35" s="226"/>
     </row>
     <row r="36" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="181" t="s">
+      <c r="A36" s="227" t="s">
         <v>342</v>
       </c>
-      <c r="B36" s="182" t="s">
+      <c r="B36" s="228" t="s">
         <v>343</v>
       </c>
-      <c r="C36" s="183"/>
-      <c r="D36" s="170" t="s">
+      <c r="C36" s="229"/>
+      <c r="D36" s="235" t="s">
         <v>351</v>
       </c>
-      <c r="E36" s="171"/>
-      <c r="F36" s="170" t="s">
+      <c r="E36" s="236"/>
+      <c r="F36" s="235" t="s">
         <v>345</v>
       </c>
-      <c r="G36" s="171"/>
-      <c r="H36" s="170" t="s">
+      <c r="G36" s="236"/>
+      <c r="H36" s="235" t="s">
         <v>352</v>
       </c>
-      <c r="I36" s="171"/>
-      <c r="J36" s="170" t="s">
+      <c r="I36" s="236"/>
+      <c r="J36" s="235" t="s">
         <v>353</v>
       </c>
-      <c r="K36" s="171"/>
-      <c r="V36" s="186">
+      <c r="K36" s="236"/>
+      <c r="V36" s="232">
         <f>+V26</f>
         <v>2020</v>
       </c>
-      <c r="W36" s="176"/>
-      <c r="X36" s="176">
+      <c r="W36" s="233"/>
+      <c r="X36" s="233">
         <f>+V36+1</f>
         <v>2021</v>
       </c>
-      <c r="Y36" s="176"/>
-      <c r="Z36" s="176">
+      <c r="Y36" s="233"/>
+      <c r="Z36" s="233">
         <f t="shared" ref="Z36" si="46">+X36+1</f>
         <v>2022</v>
       </c>
-      <c r="AA36" s="176"/>
-      <c r="AB36" s="176">
+      <c r="AA36" s="233"/>
+      <c r="AB36" s="233">
         <f t="shared" ref="AB36" si="47">+Z36+1</f>
         <v>2023</v>
       </c>
-      <c r="AC36" s="176"/>
-      <c r="AD36" s="176">
+      <c r="AC36" s="233"/>
+      <c r="AD36" s="233">
         <f t="shared" ref="AD36" si="48">+AB36+1</f>
         <v>2024</v>
       </c>
-      <c r="AE36" s="176"/>
-      <c r="AF36" s="176">
+      <c r="AE36" s="233"/>
+      <c r="AF36" s="233">
         <f t="shared" ref="AF36" si="49">+AD36+1</f>
         <v>2025</v>
       </c>
-      <c r="AG36" s="176"/>
-      <c r="AH36" s="176">
+      <c r="AG36" s="233"/>
+      <c r="AH36" s="233">
         <f t="shared" ref="AH36" si="50">+AF36+1</f>
         <v>2026</v>
       </c>
-      <c r="AI36" s="176"/>
-      <c r="AJ36" s="176">
+      <c r="AI36" s="233"/>
+      <c r="AJ36" s="233">
         <f t="shared" ref="AJ36" si="51">+AH36+1</f>
         <v>2027</v>
       </c>
-      <c r="AK36" s="176"/>
-      <c r="AL36" s="176">
+      <c r="AK36" s="233"/>
+      <c r="AL36" s="233">
         <f t="shared" ref="AL36" si="52">+AJ36+1</f>
         <v>2028</v>
       </c>
-      <c r="AM36" s="176"/>
-      <c r="AN36" s="176">
+      <c r="AM36" s="233"/>
+      <c r="AN36" s="233">
         <f t="shared" ref="AN36" si="53">+AL36+1</f>
         <v>2029</v>
       </c>
-      <c r="AO36" s="176"/>
-      <c r="AP36" s="176">
+      <c r="AO36" s="233"/>
+      <c r="AP36" s="233">
         <f t="shared" ref="AP36" si="54">+AN36+1</f>
         <v>2030</v>
       </c>
-      <c r="AQ36" s="176"/>
-      <c r="AR36" s="176">
+      <c r="AQ36" s="233"/>
+      <c r="AR36" s="233">
         <f t="shared" ref="AR36" si="55">+AP36+1</f>
         <v>2031</v>
       </c>
-      <c r="AS36" s="176"/>
-      <c r="AT36" s="176">
+      <c r="AS36" s="233"/>
+      <c r="AT36" s="233">
         <f t="shared" ref="AT36" si="56">+AR36+1</f>
         <v>2032</v>
       </c>
-      <c r="AU36" s="177"/>
+      <c r="AU36" s="234"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A37" s="181"/>
-      <c r="B37" s="184"/>
-      <c r="C37" s="185"/>
-      <c r="D37" s="172"/>
-      <c r="E37" s="173"/>
-      <c r="F37" s="172"/>
-      <c r="G37" s="173"/>
-      <c r="H37" s="172"/>
-      <c r="I37" s="173"/>
-      <c r="J37" s="172"/>
-      <c r="K37" s="173"/>
+      <c r="A37" s="227"/>
+      <c r="B37" s="230"/>
+      <c r="C37" s="231"/>
+      <c r="D37" s="237"/>
+      <c r="E37" s="238"/>
+      <c r="F37" s="237"/>
+      <c r="G37" s="238"/>
+      <c r="H37" s="237"/>
+      <c r="I37" s="238"/>
+      <c r="J37" s="237"/>
+      <c r="K37" s="238"/>
       <c r="V37" s="102" t="s">
         <v>280</v>
       </c>
@@ -11576,11 +12100,11 @@
       </c>
     </row>
     <row r="38" spans="1:47" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="181"/>
-      <c r="B38" s="174" t="s">
+      <c r="A38" s="227"/>
+      <c r="B38" s="205" t="s">
         <v>280</v>
       </c>
-      <c r="C38" s="175"/>
+      <c r="C38" s="206"/>
       <c r="D38" s="118">
         <f>+E27/$E$27</f>
         <v>1</v>
@@ -11666,11 +12190,11 @@
       <c r="AU38" s="105"/>
     </row>
     <row r="39" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="181"/>
-      <c r="B39" s="174" t="s">
+      <c r="A39" s="227"/>
+      <c r="B39" s="205" t="s">
         <v>281</v>
       </c>
-      <c r="C39" s="175"/>
+      <c r="C39" s="206"/>
       <c r="D39" s="118">
         <f>+F28/$E$27</f>
         <v>0.83333333333333337</v>
@@ -11768,11 +12292,11 @@
       </c>
     </row>
     <row r="40" spans="1:47" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="181"/>
-      <c r="B40" s="174" t="s">
+      <c r="A40" s="227"/>
+      <c r="B40" s="205" t="s">
         <v>282</v>
       </c>
-      <c r="C40" s="175"/>
+      <c r="C40" s="206"/>
       <c r="D40" s="118">
         <f>+G29/$E$27</f>
         <v>0.83333333333333337</v>
@@ -11867,11 +12391,11 @@
       <c r="AU40" s="105"/>
     </row>
     <row r="41" spans="1:47" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="181"/>
-      <c r="B41" s="174" t="s">
+      <c r="A41" s="227"/>
+      <c r="B41" s="205" t="s">
         <v>283</v>
       </c>
-      <c r="C41" s="175"/>
+      <c r="C41" s="206"/>
       <c r="D41" s="118">
         <f>+H30/$E$27</f>
         <v>0.83333333333333337</v>
@@ -11963,11 +12487,11 @@
       </c>
     </row>
     <row r="42" spans="1:47" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="181"/>
-      <c r="B42" s="174" t="s">
+      <c r="A42" s="227"/>
+      <c r="B42" s="205" t="s">
         <v>284</v>
       </c>
-      <c r="C42" s="175"/>
+      <c r="C42" s="206"/>
       <c r="D42" s="118">
         <f>+I31/$E$27</f>
         <v>0.75</v>
@@ -12056,11 +12580,11 @@
       <c r="AU42" s="105"/>
     </row>
     <row r="43" spans="1:47" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="181"/>
-      <c r="B43" s="174" t="s">
+      <c r="A43" s="227"/>
+      <c r="B43" s="205" t="s">
         <v>285</v>
       </c>
-      <c r="C43" s="175"/>
+      <c r="C43" s="206"/>
       <c r="D43" s="124">
         <f>+J32/$E$27</f>
         <v>0.75</v>
@@ -12150,44 +12674,47 @@
     </row>
   </sheetData>
   <mergeCells count="95">
-    <mergeCell ref="V2:AS2"/>
-    <mergeCell ref="A3:B4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AR3:AS3"/>
-    <mergeCell ref="AT3:AU3"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="V13:AU13"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AT14:AU14"/>
-    <mergeCell ref="X14:Y14"/>
-    <mergeCell ref="Z14:AA14"/>
-    <mergeCell ref="AB14:AC14"/>
-    <mergeCell ref="AD14:AE14"/>
-    <mergeCell ref="AF14:AG14"/>
-    <mergeCell ref="AH14:AI14"/>
-    <mergeCell ref="AJ14:AK14"/>
-    <mergeCell ref="AL14:AM14"/>
-    <mergeCell ref="AN14:AO14"/>
-    <mergeCell ref="AP14:AQ14"/>
-    <mergeCell ref="AR14:AS14"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="AN36:AO36"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="D36:E37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="H36:I37"/>
+    <mergeCell ref="J36:K37"/>
+    <mergeCell ref="AJ36:AK36"/>
+    <mergeCell ref="AL36:AM36"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="V35:AU35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="B36:C37"/>
+    <mergeCell ref="V36:W36"/>
+    <mergeCell ref="X36:Y36"/>
+    <mergeCell ref="Z36:AA36"/>
+    <mergeCell ref="AP36:AQ36"/>
+    <mergeCell ref="AR36:AS36"/>
+    <mergeCell ref="AT36:AU36"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="AB36:AC36"/>
+    <mergeCell ref="AD36:AE36"/>
+    <mergeCell ref="AF36:AG36"/>
+    <mergeCell ref="AH36:AI36"/>
+    <mergeCell ref="AT26:AU26"/>
+    <mergeCell ref="X26:Y26"/>
+    <mergeCell ref="Z26:AA26"/>
+    <mergeCell ref="AB26:AC26"/>
+    <mergeCell ref="AD26:AE26"/>
+    <mergeCell ref="AF26:AG26"/>
+    <mergeCell ref="AH26:AI26"/>
+    <mergeCell ref="AJ26:AK26"/>
+    <mergeCell ref="AL26:AM26"/>
+    <mergeCell ref="AN26:AO26"/>
+    <mergeCell ref="AP26:AQ26"/>
+    <mergeCell ref="AR26:AS26"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="V25:AU25"/>
@@ -12204,47 +12731,44 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="V14:W14"/>
-    <mergeCell ref="AT26:AU26"/>
-    <mergeCell ref="X26:Y26"/>
-    <mergeCell ref="Z26:AA26"/>
-    <mergeCell ref="AB26:AC26"/>
-    <mergeCell ref="AD26:AE26"/>
-    <mergeCell ref="AF26:AG26"/>
-    <mergeCell ref="AH26:AI26"/>
-    <mergeCell ref="AJ26:AK26"/>
-    <mergeCell ref="AL26:AM26"/>
-    <mergeCell ref="AN26:AO26"/>
-    <mergeCell ref="AP26:AQ26"/>
-    <mergeCell ref="AR26:AS26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="V35:AU35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="B36:C37"/>
-    <mergeCell ref="V36:W36"/>
-    <mergeCell ref="X36:Y36"/>
-    <mergeCell ref="Z36:AA36"/>
-    <mergeCell ref="AP36:AQ36"/>
-    <mergeCell ref="AR36:AS36"/>
-    <mergeCell ref="AT36:AU36"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="AB36:AC36"/>
-    <mergeCell ref="AD36:AE36"/>
-    <mergeCell ref="AF36:AG36"/>
-    <mergeCell ref="AH36:AI36"/>
-    <mergeCell ref="AJ36:AK36"/>
-    <mergeCell ref="AL36:AM36"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="AN36:AO36"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M25:N25"/>
-    <mergeCell ref="D36:E37"/>
-    <mergeCell ref="F36:G37"/>
-    <mergeCell ref="H36:I37"/>
-    <mergeCell ref="J36:K37"/>
+    <mergeCell ref="AT14:AU14"/>
+    <mergeCell ref="X14:Y14"/>
+    <mergeCell ref="Z14:AA14"/>
+    <mergeCell ref="AB14:AC14"/>
+    <mergeCell ref="AD14:AE14"/>
+    <mergeCell ref="AF14:AG14"/>
+    <mergeCell ref="AH14:AI14"/>
+    <mergeCell ref="AJ14:AK14"/>
+    <mergeCell ref="AL14:AM14"/>
+    <mergeCell ref="AN14:AO14"/>
+    <mergeCell ref="AP14:AQ14"/>
+    <mergeCell ref="AR14:AS14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AT3:AU3"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="V13:AU13"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="V2:AS2"/>
+    <mergeCell ref="A3:B4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AR3:AS3"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>